<commit_message>
Need to put back in original file for repository tracking sake.
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2014 data/BogLower5-R3 and R4.xlsx
+++ b/Data/phenotypic data/RawData/2014 data/BogLower5-R3 and R4.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6439" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6428" uniqueCount="217">
   <si>
     <t>Date measured:</t>
   </si>
@@ -455,6 +455,9 @@
     <t>c</t>
   </si>
   <si>
+    <t>s</t>
+  </si>
+  <si>
     <t>R/FUR</t>
   </si>
   <si>
@@ -477,6 +480,9 @@
   </si>
   <si>
     <t>4.793*</t>
+  </si>
+  <si>
+    <t>MS</t>
   </si>
   <si>
     <t>2.89*</t>
@@ -653,6 +659,9 @@
     <t>*Empty bag</t>
   </si>
   <si>
+    <t>E</t>
+  </si>
+  <si>
     <t>6.09*</t>
   </si>
   <si>
@@ -666,6 +675,9 @@
   </si>
   <si>
     <t>Date measured: 11/15/14</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>FUR/P</t>
@@ -1312,34 +1324,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:V1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K513" workbookViewId="0">
-      <selection activeCell="V532" sqref="V532"/>
+    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA534" sqref="AA534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" customWidth="1"/>
-    <col min="8" max="8" width="6.5" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" customWidth="1"/>
-    <col min="12" max="12" width="5" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" customWidth="1"/>
-    <col min="14" max="14" width="4.83203125" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" customWidth="1"/>
-    <col min="16" max="16" width="6.5" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="7.1640625" customWidth="1"/>
-    <col min="19" max="19" width="7.6640625" customWidth="1"/>
-    <col min="20" max="20" width="6.5" customWidth="1"/>
-    <col min="21" max="21" width="5.83203125" customWidth="1"/>
-    <col min="22" max="22" width="8.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="3" spans="1:22" ht="15">
       <c r="A3" s="1" t="s">
@@ -1348,7 +1338,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1623,7 +1613,7 @@
         <v>2.6</v>
       </c>
       <c r="I9" s="22">
-        <v>0</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="J9" s="34"/>
       <c r="K9" s="34">
@@ -1689,7 +1679,7 @@
         <v>4.7</v>
       </c>
       <c r="I10" s="22">
-        <v>0</v>
+        <v>20.9</v>
       </c>
       <c r="J10" s="34"/>
       <c r="K10" s="34">
@@ -1755,7 +1745,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I11" s="22">
-        <v>0</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J11" s="34"/>
       <c r="K11" s="34">
@@ -1821,7 +1811,7 @@
         <v>2.7</v>
       </c>
       <c r="I12" s="22">
-        <v>0</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="J12" s="34"/>
       <c r="K12" s="34">
@@ -1884,10 +1874,10 @@
         <v>2.52</v>
       </c>
       <c r="H13" s="22">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="I13" s="22">
-        <v>0</v>
+        <v>15.6</v>
       </c>
       <c r="J13" s="34"/>
       <c r="K13" s="34">
@@ -1953,7 +1943,7 @@
         <v>1.3</v>
       </c>
       <c r="I14" s="22">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="J14" s="34"/>
       <c r="K14" s="34">
@@ -2013,13 +2003,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H15" s="22">
         <v>2.9</v>
       </c>
       <c r="I15" s="38">
-        <v>0</v>
+        <v>18.2</v>
       </c>
       <c r="J15" s="34"/>
       <c r="K15" s="34">
@@ -2079,13 +2069,13 @@
         <v>2</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H16" s="22">
         <v>1.9</v>
       </c>
       <c r="I16" s="22">
-        <v>0</v>
+        <v>19.8</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34">
@@ -2151,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="22">
-        <v>0</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="J17" s="34"/>
       <c r="K17" s="34">
@@ -2217,7 +2207,7 @@
         <v>2.7</v>
       </c>
       <c r="I18" s="22">
-        <v>1.7</v>
+        <v>20.6</v>
       </c>
       <c r="J18" s="34"/>
       <c r="K18" s="34">
@@ -2387,13 +2377,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="22">
         <v>0</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H22" s="22">
         <v>4</v>
@@ -2421,7 +2411,7 @@
         <v>119</v>
       </c>
       <c r="Q22" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R22" s="22" t="s">
         <v>123</v>
@@ -2585,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="22">
         <v>2</v>
@@ -2651,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="22">
         <v>1</v>
@@ -2685,7 +2675,7 @@
         <v>122</v>
       </c>
       <c r="Q26" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R26" s="22" t="s">
         <v>124</v>
@@ -2849,13 +2839,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="22">
         <v>1</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H29" s="22">
         <v>2.2999999999999998</v>
@@ -2883,7 +2873,7 @@
         <v>122</v>
       </c>
       <c r="Q29" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R29" s="22" t="s">
         <v>124</v>
@@ -2974,7 +2964,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -3742,7 +3732,7 @@
         <v>1</v>
       </c>
       <c r="T45" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U45" s="34">
         <v>7</v>
@@ -4603,7 +4593,7 @@
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -4966,7 +4956,7 @@
         <v>119</v>
       </c>
       <c r="Q68" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R68" s="22" t="s">
         <v>124</v>
@@ -5004,7 +4994,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H69" s="22">
         <v>2.4</v>
@@ -5032,7 +5022,7 @@
         <v>129</v>
       </c>
       <c r="Q69" s="22" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="R69" s="22" t="s">
         <v>124</v>
@@ -5098,7 +5088,7 @@
         <v>129</v>
       </c>
       <c r="Q70" s="22" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="R70" s="22" t="s">
         <v>124</v>
@@ -5136,7 +5126,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="22" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H71" s="22">
         <v>0</v>
@@ -5296,7 +5286,7 @@
         <v>129</v>
       </c>
       <c r="Q73" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R73" s="22" t="s">
         <v>124</v>
@@ -5466,7 +5456,7 @@
         <v>0</v>
       </c>
       <c r="G76" s="22" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H76" s="22">
         <v>4.2</v>
@@ -5494,7 +5484,7 @@
         <v>119</v>
       </c>
       <c r="Q76" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R76" s="22" t="s">
         <v>124</v>
@@ -5678,7 +5668,7 @@
         <v>119</v>
       </c>
       <c r="Q80" s="22" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="R80" s="22" t="s">
         <v>124</v>
@@ -5965,7 +5955,7 @@
         <v>7</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C85" s="22"/>
       <c r="D85" s="22"/>
@@ -6196,7 +6186,7 @@
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -6600,7 +6590,7 @@
         <v>3.16</v>
       </c>
       <c r="H98" s="22">
-        <v>2.1</v>
+        <v>21</v>
       </c>
       <c r="I98" s="22">
         <v>0</v>
@@ -6795,7 +6785,7 @@
         <v>1</v>
       </c>
       <c r="G101" s="22" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H101" s="22">
         <v>4.8</v>
@@ -7822,7 +7812,7 @@
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
@@ -8317,7 +8307,7 @@
         <v>119</v>
       </c>
       <c r="Q128" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R128" s="22" t="s">
         <v>124</v>
@@ -8710,7 +8700,7 @@
         <v>138</v>
       </c>
       <c r="P134" s="37" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="Q134" s="22" t="s">
         <v>124</v>
@@ -10785,7 +10775,7 @@
         <v>119</v>
       </c>
       <c r="Q171" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R171" s="22" t="s">
         <v>124</v>
@@ -10917,7 +10907,7 @@
         <v>119</v>
       </c>
       <c r="Q173" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R173" s="22" t="s">
         <v>124</v>
@@ -10983,7 +10973,7 @@
         <v>122</v>
       </c>
       <c r="Q174" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R174" s="22" t="s">
         <v>124</v>
@@ -14271,7 +14261,7 @@
         <v>0</v>
       </c>
       <c r="G233" s="22" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="H233" s="22">
         <v>5</v>
@@ -15821,7 +15811,7 @@
         <v>2</v>
       </c>
       <c r="G261" s="22">
-        <v>7.78</v>
+        <v>7078</v>
       </c>
       <c r="H261" s="22">
         <v>5</v>
@@ -15852,7 +15842,7 @@
         <v>124</v>
       </c>
       <c r="R261" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="S261" s="34">
         <v>1</v>
@@ -15940,7 +15930,7 @@
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E264" s="3"/>
       <c r="F264" s="3"/>
@@ -16288,7 +16278,7 @@
         <v>17.2</v>
       </c>
       <c r="L271" s="34">
-        <v>14.8</v>
+        <v>41.8</v>
       </c>
       <c r="M271" s="34">
         <v>1.651</v>
@@ -17079,7 +17069,7 @@
         <v>129</v>
       </c>
       <c r="Q284" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R284" s="22" t="s">
         <v>124</v>
@@ -17343,7 +17333,7 @@
         <v>119</v>
       </c>
       <c r="Q288" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R288" s="22" t="s">
         <v>124</v>
@@ -17475,7 +17465,7 @@
         <v>119</v>
       </c>
       <c r="Q290" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R290" s="22" t="s">
         <v>124</v>
@@ -17566,7 +17556,7 @@
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E293" s="3"/>
       <c r="F293" s="3"/>
@@ -18448,7 +18438,7 @@
         <v>2.06</v>
       </c>
       <c r="N308" s="35">
-        <v>2.7</v>
+        <v>2.06</v>
       </c>
       <c r="O308" s="37" t="s">
         <v>119</v>
@@ -18837,7 +18827,7 @@
         <v>122</v>
       </c>
       <c r="Q315" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R315" s="22" t="s">
         <v>131</v>
@@ -18846,7 +18836,7 @@
         <v>1</v>
       </c>
       <c r="T315" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U315" s="34">
         <v>18</v>
@@ -19110,7 +19100,7 @@
         <v>1</v>
       </c>
       <c r="T319" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U319" s="34">
         <v>28</v>
@@ -19624,7 +19614,7 @@
         <v>124</v>
       </c>
       <c r="R330" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S330" s="34">
         <v>3</v>
@@ -20213,9 +20203,7 @@
       <c r="U340" s="34">
         <v>25</v>
       </c>
-      <c r="V340" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V340" s="22"/>
     </row>
     <row r="341" spans="1:22">
       <c r="A341" s="4">
@@ -20279,9 +20267,7 @@
       <c r="U341" s="34">
         <v>29</v>
       </c>
-      <c r="V341" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V341" s="22"/>
     </row>
     <row r="342" spans="1:22">
       <c r="A342" s="4">
@@ -20345,9 +20331,7 @@
       <c r="U342" s="34">
         <v>10</v>
       </c>
-      <c r="V342" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V342" s="22"/>
     </row>
     <row r="343" spans="1:22">
       <c r="A343" s="4">
@@ -20411,9 +20395,7 @@
       <c r="U343" s="34">
         <v>19</v>
       </c>
-      <c r="V343" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V343" s="22"/>
     </row>
     <row r="344" spans="1:22">
       <c r="A344" s="4">
@@ -20477,9 +20459,7 @@
       <c r="U344" s="34">
         <v>13</v>
       </c>
-      <c r="V344" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V344" s="22"/>
     </row>
     <row r="345" spans="1:22">
       <c r="A345" s="4">
@@ -20543,9 +20523,7 @@
       <c r="U345" s="34">
         <v>20</v>
       </c>
-      <c r="V345" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V345" s="22"/>
     </row>
     <row r="346" spans="1:22">
       <c r="A346" s="4">
@@ -20609,9 +20587,7 @@
       <c r="U346" s="34">
         <v>21</v>
       </c>
-      <c r="V346" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V346" s="22"/>
     </row>
     <row r="347" spans="1:22">
       <c r="A347" s="4">
@@ -20675,9 +20651,7 @@
       <c r="U347" s="34">
         <v>22</v>
       </c>
-      <c r="V347" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V347" s="22"/>
     </row>
     <row r="348" spans="1:22">
       <c r="A348" s="4">
@@ -20741,9 +20715,7 @@
       <c r="U348" s="34">
         <v>24</v>
       </c>
-      <c r="V348" s="22" t="s">
-        <v>127</v>
-      </c>
+      <c r="V348" s="22"/>
     </row>
     <row r="349" spans="1:22">
       <c r="A349" s="4">
@@ -20793,7 +20765,7 @@
         <v>119</v>
       </c>
       <c r="Q349" s="22" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="R349" s="22" t="s">
         <v>124</v>
@@ -20807,14 +20779,9 @@
       <c r="U349" s="34">
         <v>17</v>
       </c>
-      <c r="V349" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="V349" s="22"/>
     </row>
     <row r="350" spans="1:22">
-      <c r="A350" s="4">
-        <v>11</v>
-      </c>
       <c r="B350" s="22">
         <v>5</v>
       </c>
@@ -20871,9 +20838,6 @@
       </c>
       <c r="U350" s="34">
         <v>15</v>
-      </c>
-      <c r="V350" s="22" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="351" spans="1:22" ht="15">
@@ -21180,7 +21144,7 @@
         <v>119</v>
       </c>
       <c r="Q357" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R357" s="22" t="s">
         <v>124</v>
@@ -21246,7 +21210,7 @@
         <v>119</v>
       </c>
       <c r="Q358" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R358" s="22" t="s">
         <v>124</v>
@@ -21312,7 +21276,7 @@
         <v>119</v>
       </c>
       <c r="Q359" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R359" s="22" t="s">
         <v>124</v>
@@ -21378,7 +21342,7 @@
         <v>119</v>
       </c>
       <c r="Q360" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R360" s="22" t="s">
         <v>124</v>
@@ -21444,7 +21408,7 @@
         <v>119</v>
       </c>
       <c r="Q361" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R361" s="22" t="s">
         <v>131</v>
@@ -21510,7 +21474,7 @@
         <v>119</v>
       </c>
       <c r="Q362" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R362" s="22" t="s">
         <v>124</v>
@@ -21519,7 +21483,7 @@
         <v>2</v>
       </c>
       <c r="T362" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U362" s="34">
         <v>21</v>
@@ -21576,7 +21540,7 @@
         <v>119</v>
       </c>
       <c r="Q363" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R363" s="22" t="s">
         <v>124</v>
@@ -21642,7 +21606,7 @@
         <v>119</v>
       </c>
       <c r="Q364" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R364" s="22" t="s">
         <v>124</v>
@@ -21708,7 +21672,7 @@
         <v>122</v>
       </c>
       <c r="Q365" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R365" s="22" t="s">
         <v>124</v>
@@ -21783,7 +21747,7 @@
         <v>1</v>
       </c>
       <c r="T366" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U366" s="34">
         <v>9</v>
@@ -22509,7 +22473,7 @@
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E380" s="3"/>
       <c r="F380" s="3"/>
@@ -24135,7 +24099,7 @@
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
       <c r="D409" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E409" s="3"/>
       <c r="F409" s="3"/>
@@ -24696,7 +24660,7 @@
         <v>120</v>
       </c>
       <c r="Q419" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R419" s="22" t="s">
         <v>124</v>
@@ -25026,7 +24990,7 @@
         <v>122</v>
       </c>
       <c r="Q424" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R424" s="22" t="s">
         <v>124</v>
@@ -25157,7 +25121,7 @@
         <v>16</v>
       </c>
       <c r="V427" s="22" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
     </row>
     <row r="428" spans="1:22">
@@ -25223,7 +25187,7 @@
         <v>24</v>
       </c>
       <c r="V428" s="22" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
     </row>
     <row r="429" spans="1:22">
@@ -25421,7 +25385,7 @@
         <v>17</v>
       </c>
       <c r="V431" s="22" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
     </row>
     <row r="432" spans="1:22">
@@ -25487,7 +25451,7 @@
         <v>10</v>
       </c>
       <c r="V432" s="22" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
     </row>
     <row r="433" spans="1:22">
@@ -25761,7 +25725,7 @@
       <c r="B438" s="2"/>
       <c r="C438" s="2"/>
       <c r="D438" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E438" s="3"/>
       <c r="F438" s="3"/>
@@ -26127,7 +26091,7 @@
         <v>124</v>
       </c>
       <c r="R445" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S445">
         <v>1</v>
@@ -26589,7 +26553,7 @@
         <v>124</v>
       </c>
       <c r="R452" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S452">
         <v>1</v>
@@ -27387,7 +27351,7 @@
       <c r="B467" s="2"/>
       <c r="C467" s="2"/>
       <c r="D467" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E467" s="3"/>
       <c r="F467" s="3"/>
@@ -27684,7 +27648,7 @@
         <v>119</v>
       </c>
       <c r="Q473" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R473" s="22" t="s">
         <v>124</v>
@@ -27816,7 +27780,7 @@
         <v>119</v>
       </c>
       <c r="Q475" s="22" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="R475" s="22" t="s">
         <v>124</v>
@@ -27825,7 +27789,7 @@
         <v>1</v>
       </c>
       <c r="T475" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U475" s="34">
         <v>20</v>
@@ -28023,7 +27987,7 @@
         <v>1</v>
       </c>
       <c r="T478" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U478" s="34">
         <v>15</v>
@@ -28155,7 +28119,7 @@
         <v>1</v>
       </c>
       <c r="T480" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U480" s="34">
         <v>9</v>
@@ -28221,7 +28185,7 @@
         <v>2</v>
       </c>
       <c r="T481" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U481" s="34">
         <v>14</v>
@@ -28278,7 +28242,7 @@
         <v>122</v>
       </c>
       <c r="Q482" s="22" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="R482" s="22" t="s">
         <v>124</v>
@@ -28287,7 +28251,7 @@
         <v>2</v>
       </c>
       <c r="T482" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U482" s="34">
         <v>15</v>
@@ -28471,7 +28435,7 @@
         <v>121</v>
       </c>
       <c r="U486" s="34">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="V486" s="22" t="s">
         <v>127</v>
@@ -28566,7 +28530,7 @@
         <v>4.29</v>
       </c>
       <c r="H488" s="22">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="I488" s="22">
         <v>0</v>
@@ -29012,7 +28976,7 @@
       <c r="B496" s="2"/>
       <c r="C496" s="2"/>
       <c r="D496" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E496" s="3"/>
       <c r="F496" s="3"/>
@@ -29450,7 +29414,7 @@
         <v>1</v>
       </c>
       <c r="T504" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U504" s="34">
         <v>8</v>
@@ -29714,7 +29678,7 @@
         <v>1</v>
       </c>
       <c r="T508" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U508" s="34">
         <v>25</v>
@@ -29825,7 +29789,7 @@
         <v>16.3</v>
       </c>
       <c r="M510" s="34">
-        <v>2.3199999999999998</v>
+        <v>2.31</v>
       </c>
       <c r="N510" s="35">
         <v>3.3</v>
@@ -30490,7 +30454,7 @@
         <v>1</v>
       </c>
       <c r="T521" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U521" s="34">
         <v>16</v>
@@ -30863,7 +30827,7 @@
     </row>
     <row r="530" spans="1:22">
       <c r="A530" s="28" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B530" s="29"/>
       <c r="C530" s="29"/>
@@ -31334,7 +31298,7 @@
         <v>124</v>
       </c>
       <c r="R537" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S537" s="34">
         <v>1</v>
@@ -35849,13 +35813,13 @@
         <v>2.9</v>
       </c>
       <c r="O618" s="36" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P618" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q618" s="22" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
       <c r="R618" s="22" t="s">
         <v>124</v>
@@ -35915,10 +35879,10 @@
         <v>3.7</v>
       </c>
       <c r="O619" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P619" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q619" s="22" t="s">
         <v>123</v>
@@ -35959,7 +35923,7 @@
         <v>6</v>
       </c>
       <c r="G620" s="22">
-        <v>2.5209999999999999</v>
+        <v>2.3210000000000002</v>
       </c>
       <c r="H620" s="22">
         <v>3.1</v>
@@ -35981,10 +35945,10 @@
         <v>3.3</v>
       </c>
       <c r="O620" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P620" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q620" s="22" t="s">
         <v>123</v>
@@ -36047,10 +36011,10 @@
         <v>3.1</v>
       </c>
       <c r="O621" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P621" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q621" s="22" t="s">
         <v>123</v>
@@ -36113,10 +36077,10 @@
         <v>3</v>
       </c>
       <c r="O622" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P622" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="Q622" s="22" t="s">
         <v>125</v>
@@ -36179,10 +36143,10 @@
         <v>2.9</v>
       </c>
       <c r="O623" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P623" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="Q623" s="22" t="s">
         <v>123</v>
@@ -36245,10 +36209,10 @@
         <v>2.8</v>
       </c>
       <c r="O624" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P624" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="Q624" s="22" t="s">
         <v>123</v>
@@ -36311,10 +36275,10 @@
         <v>3.1</v>
       </c>
       <c r="O625" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P625" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q625" s="22" t="s">
         <v>125</v>
@@ -36377,10 +36341,10 @@
         <v>2.8</v>
       </c>
       <c r="O626" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P626" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="Q626" s="22" t="s">
         <v>123</v>
@@ -36443,16 +36407,16 @@
         <v>3.5</v>
       </c>
       <c r="O627" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P627" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q627" s="22" t="s">
         <v>125</v>
       </c>
       <c r="R627" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="S627" s="34">
         <v>2</v>
@@ -36565,7 +36529,7 @@
         <v>119</v>
       </c>
       <c r="Q630" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R630" s="22" t="s">
         <v>131</v>
@@ -36829,7 +36793,7 @@
         <v>122</v>
       </c>
       <c r="Q634" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R634" s="22" t="s">
         <v>124</v>
@@ -37184,7 +37148,7 @@
       <c r="B641" s="2"/>
       <c r="C641" s="2"/>
       <c r="D641" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E641" s="3"/>
       <c r="F641" s="3"/>
@@ -37556,7 +37520,7 @@
         <v>2</v>
       </c>
       <c r="T648" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U648" s="34">
         <v>6</v>
@@ -37595,7 +37559,7 @@
       </c>
       <c r="J649" s="34"/>
       <c r="K649" s="34">
-        <v>19.399999999999999</v>
+        <v>1.94</v>
       </c>
       <c r="L649" s="34">
         <v>15.6</v>
@@ -37622,7 +37586,7 @@
         <v>2</v>
       </c>
       <c r="T649" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U649" s="34">
         <v>3</v>
@@ -37688,7 +37652,7 @@
         <v>1</v>
       </c>
       <c r="T650" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U650" s="34">
         <v>10</v>
@@ -37754,7 +37718,7 @@
         <v>2</v>
       </c>
       <c r="T651" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U651" s="34">
         <v>10</v>
@@ -37952,7 +37916,7 @@
         <v>2</v>
       </c>
       <c r="T654" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U654" s="34">
         <v>6</v>
@@ -38018,7 +37982,7 @@
         <v>3</v>
       </c>
       <c r="T655" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U655" s="34">
         <v>16</v>
@@ -38101,9 +38065,7 @@
       <c r="E657" s="11"/>
       <c r="F657" s="11"/>
       <c r="G657" s="11"/>
-      <c r="H657" s="11">
-        <v>3.9</v>
-      </c>
+      <c r="H657" s="11"/>
       <c r="I657" s="11"/>
       <c r="J657" s="16"/>
       <c r="K657" s="16"/>
@@ -38448,7 +38410,7 @@
         <v>3.508</v>
       </c>
       <c r="N663" s="35">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
       <c r="O663" s="37" t="s">
         <v>119</v>
@@ -38812,7 +38774,7 @@
       <c r="B670" s="2"/>
       <c r="C670" s="2"/>
       <c r="D670" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E670" s="3"/>
       <c r="F670" s="3"/>
@@ -39729,9 +39691,7 @@
       <c r="E686" s="11"/>
       <c r="F686" s="11"/>
       <c r="G686" s="11"/>
-      <c r="H686" s="11">
-        <v>2.4</v>
-      </c>
+      <c r="H686" s="11"/>
       <c r="I686" s="11"/>
       <c r="J686" s="16"/>
       <c r="K686" s="16"/>
@@ -39925,7 +39885,7 @@
         <v>0</v>
       </c>
       <c r="G690" s="22">
-        <v>4.6420000000000003</v>
+        <v>4.0419999999999998</v>
       </c>
       <c r="H690" s="22">
         <v>2.4</v>
@@ -40067,7 +40027,7 @@
       </c>
       <c r="J692" s="34"/>
       <c r="K692" s="34">
-        <v>24.6</v>
+        <v>21.4</v>
       </c>
       <c r="L692" s="34">
         <v>19.899999999999999</v>
@@ -40349,7 +40309,7 @@
         <v>119</v>
       </c>
       <c r="Q696" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R696" s="22" t="s">
         <v>124</v>
@@ -40440,7 +40400,7 @@
       <c r="B699" s="2"/>
       <c r="C699" s="2"/>
       <c r="D699" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E699" s="3"/>
       <c r="F699" s="3"/>
@@ -41419,7 +41379,7 @@
         <v>3</v>
       </c>
       <c r="G717" s="22" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H717" s="22">
         <v>3.8</v>
@@ -41642,7 +41602,7 @@
         <v>120</v>
       </c>
       <c r="P720" s="37" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="Q720" s="22" t="s">
         <v>124</v>
@@ -41828,7 +41788,7 @@
         <v>23.2</v>
       </c>
       <c r="L723" s="34">
-        <v>15.9</v>
+        <v>15.7</v>
       </c>
       <c r="M723" s="34">
         <v>2.528</v>
@@ -42066,7 +42026,7 @@
       <c r="B728" s="2"/>
       <c r="C728" s="2"/>
       <c r="D728" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E728" s="3"/>
       <c r="F728" s="3"/>
@@ -42636,7 +42596,7 @@
         <v>1</v>
       </c>
       <c r="T738" s="34" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="U738" s="34">
         <v>32</v>
@@ -42702,7 +42662,7 @@
         <v>1</v>
       </c>
       <c r="T739" s="34" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="U739" s="34">
         <v>23</v>
@@ -43045,7 +43005,7 @@
         <v>2</v>
       </c>
       <c r="G746" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H746" s="22">
         <v>2.7</v>
@@ -43067,10 +43027,10 @@
         <v>2.5</v>
       </c>
       <c r="O746" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P746" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="Q746" s="22" t="s">
         <v>124</v>
@@ -43111,7 +43071,7 @@
         <v>2</v>
       </c>
       <c r="G747" s="22" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H747" s="22">
         <v>4.0999999999999996</v>
@@ -43133,10 +43093,10 @@
         <v>3.2</v>
       </c>
       <c r="O747" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P747" s="37" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="Q747" s="22" t="s">
         <v>124</v>
@@ -43199,7 +43159,7 @@
         <v>2.9</v>
       </c>
       <c r="O748" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P748" s="37" t="s">
         <v>119</v>
@@ -43265,7 +43225,7 @@
         <v>2.6</v>
       </c>
       <c r="O749" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P749" s="37" t="s">
         <v>119</v>
@@ -43322,7 +43282,7 @@
         <v>20.6</v>
       </c>
       <c r="L750" s="34">
-        <v>17.7</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="M750" s="34">
         <v>2.37</v>
@@ -43331,7 +43291,7 @@
         <v>3</v>
       </c>
       <c r="O750" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P750" s="37" t="s">
         <v>119</v>
@@ -43397,7 +43357,7 @@
         <v>2.4</v>
       </c>
       <c r="O751" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P751" s="37" t="s">
         <v>129</v>
@@ -43463,7 +43423,7 @@
         <v>2.6</v>
       </c>
       <c r="O752" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P752" s="37" t="s">
         <v>119</v>
@@ -43529,7 +43489,7 @@
         <v>2.6</v>
       </c>
       <c r="O753" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P753" s="37" t="s">
         <v>119</v>
@@ -43595,7 +43555,7 @@
         <v>3.1</v>
       </c>
       <c r="O754" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P754" s="37" t="s">
         <v>122</v>
@@ -43661,7 +43621,7 @@
         <v>2.7</v>
       </c>
       <c r="O755" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P755" s="37" t="s">
         <v>119</v>
@@ -43692,7 +43652,7 @@
       <c r="B757" s="2"/>
       <c r="C757" s="2"/>
       <c r="D757" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E757" s="3"/>
       <c r="F757" s="3"/>
@@ -43961,7 +43921,7 @@
         <v>0</v>
       </c>
       <c r="G763" s="22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H763" s="22">
         <v>4</v>
@@ -44225,7 +44185,7 @@
         <v>1</v>
       </c>
       <c r="G767" s="22" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H767" s="22">
         <v>2.5</v>
@@ -45004,7 +44964,7 @@
         <v>8.125</v>
       </c>
       <c r="H780" s="22" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I780" s="22">
         <v>0</v>
@@ -45044,7 +45004,7 @@
         <v>13</v>
       </c>
       <c r="V780" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="781" spans="1:22">
@@ -45265,7 +45225,7 @@
         <v>2</v>
       </c>
       <c r="G784" s="22" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H784" s="22">
         <v>3.9</v>
@@ -45318,7 +45278,7 @@
       <c r="B786" s="2"/>
       <c r="C786" s="2"/>
       <c r="D786" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E786" s="3"/>
       <c r="F786" s="3"/>
@@ -46319,7 +46279,7 @@
         <v>2.9</v>
       </c>
       <c r="O804" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P804" s="37" t="s">
         <v>122</v>
@@ -46385,7 +46345,7 @@
         <v>2.8</v>
       </c>
       <c r="O805" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P805" s="37" t="s">
         <v>119</v>
@@ -46445,13 +46405,13 @@
         <v>18.100000000000001</v>
       </c>
       <c r="M806" s="34">
-        <v>2.69</v>
+        <v>2.68</v>
       </c>
       <c r="N806" s="35">
         <v>3.4</v>
       </c>
       <c r="O806" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P806" s="37" t="s">
         <v>122</v>
@@ -46517,7 +46477,7 @@
         <v>3.2</v>
       </c>
       <c r="O807" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P807" s="37" t="s">
         <v>122</v>
@@ -46583,7 +46543,7 @@
         <v>2.9</v>
       </c>
       <c r="O808" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P808" s="37" t="s">
         <v>122</v>
@@ -46649,7 +46609,7 @@
         <v>3.1</v>
       </c>
       <c r="O809" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P809" s="37" t="s">
         <v>119</v>
@@ -46715,7 +46675,7 @@
         <v>3.1</v>
       </c>
       <c r="O810" s="37" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="P810" s="37" t="s">
         <v>122</v>
@@ -46769,7 +46729,7 @@
       </c>
       <c r="J811" s="34"/>
       <c r="K811" s="34">
-        <v>16.5</v>
+        <v>15.5</v>
       </c>
       <c r="L811" s="34">
         <v>16.8</v>
@@ -46781,7 +46741,7 @@
         <v>3.1</v>
       </c>
       <c r="O811" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P811" s="37" t="s">
         <v>122</v>
@@ -46847,7 +46807,7 @@
         <v>3.3</v>
       </c>
       <c r="O812" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P812" s="37" t="s">
         <v>122</v>
@@ -46891,7 +46851,7 @@
         <v>0</v>
       </c>
       <c r="G813" s="22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H813" s="11">
         <v>2.7</v>
@@ -46907,13 +46867,13 @@
         <v>14.9</v>
       </c>
       <c r="M813" s="34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="N813" s="35">
         <v>2.9</v>
       </c>
       <c r="O813" s="37" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="P813" s="37" t="s">
         <v>122</v>
@@ -46947,7 +46907,7 @@
       <c r="B815" s="2"/>
       <c r="C815" s="2"/>
       <c r="D815" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E815" s="3"/>
       <c r="F815" s="3"/>
@@ -47379,7 +47339,7 @@
         <v>123</v>
       </c>
       <c r="R823" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S823" s="34">
         <v>2</v>
@@ -47577,7 +47537,7 @@
         <v>123</v>
       </c>
       <c r="R826" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S826" s="34">
         <v>2</v>
@@ -48388,7 +48348,7 @@
         <v>1</v>
       </c>
       <c r="G840" s="22" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H840" s="22">
         <v>3.8</v>
@@ -48573,7 +48533,7 @@
       <c r="B844" s="2"/>
       <c r="C844" s="2"/>
       <c r="D844" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E844" s="3"/>
       <c r="F844" s="3"/>
@@ -48911,7 +48871,7 @@
         <v>4.6210000000000004</v>
       </c>
       <c r="H851" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I851" s="22">
         <v>0</v>
@@ -48951,7 +48911,7 @@
         <v>7</v>
       </c>
       <c r="V851" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="852" spans="1:22">
@@ -49017,7 +48977,7 @@
         <v>16</v>
       </c>
       <c r="V852" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="853" spans="1:22">
@@ -49083,7 +49043,7 @@
         <v>11</v>
       </c>
       <c r="V853" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="854" spans="1:22">
@@ -49172,7 +49132,7 @@
         <v>1</v>
       </c>
       <c r="G855" s="22" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H855" s="22">
         <v>4.0999999999999996</v>
@@ -49215,7 +49175,7 @@
         <v>11</v>
       </c>
       <c r="V855" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="856" spans="1:22">
@@ -49373,7 +49333,7 @@
         <v>6.9320000000000004</v>
       </c>
       <c r="H858" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I858" s="22">
         <v>0</v>
@@ -49413,7 +49373,7 @@
         <v>17</v>
       </c>
       <c r="V858" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="859" spans="1:22">
@@ -50199,7 +50159,7 @@
       <c r="B873" s="2"/>
       <c r="C873" s="2"/>
       <c r="D873" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E873" s="3"/>
       <c r="F873" s="3"/>
@@ -50930,7 +50890,7 @@
         <v>0</v>
       </c>
       <c r="G886" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H886" s="22">
         <v>4.5</v>
@@ -50946,7 +50906,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="M886" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="N886" s="22">
         <v>2.8</v>
@@ -51442,7 +51402,7 @@
         <v>1</v>
       </c>
       <c r="G895" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H895" s="22">
         <v>4.8</v>
@@ -51828,7 +51788,7 @@
       <c r="B902" s="2"/>
       <c r="C902" s="2"/>
       <c r="D902" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E902" s="3"/>
       <c r="F902" s="3"/>
@@ -52100,7 +52060,7 @@
         <v>6.48</v>
       </c>
       <c r="H908" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I908" s="22">
         <v>0</v>
@@ -52191,7 +52151,7 @@
         <v>122</v>
       </c>
       <c r="Q909" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R909" s="22" t="s">
         <v>123</v>
@@ -52245,7 +52205,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="M910" s="34">
-        <v>2.16</v>
+        <v>1.26</v>
       </c>
       <c r="N910" s="35">
         <v>3</v>
@@ -53093,7 +53053,7 @@
         <v>3</v>
       </c>
       <c r="O924" s="37" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="P924" s="37" t="s">
         <v>122</v>
@@ -53454,7 +53414,7 @@
       <c r="B931" s="2"/>
       <c r="C931" s="2"/>
       <c r="D931" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E931" s="3"/>
       <c r="F931" s="3"/>
@@ -54427,7 +54387,7 @@
         <v>2</v>
       </c>
       <c r="E949" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F949" s="22">
         <v>3</v>
@@ -54493,7 +54453,7 @@
         <v>2</v>
       </c>
       <c r="E950" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F950" s="22">
         <v>1</v>
@@ -54559,7 +54519,7 @@
         <v>2</v>
       </c>
       <c r="E951" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F951" s="22">
         <v>4</v>
@@ -54625,7 +54585,7 @@
         <v>4</v>
       </c>
       <c r="E952" s="22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F952" s="22">
         <v>3</v>
@@ -54691,7 +54651,7 @@
         <v>2</v>
       </c>
       <c r="E953" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F953" s="22">
         <v>1</v>
@@ -54757,7 +54717,7 @@
         <v>3</v>
       </c>
       <c r="E954" s="22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F954" s="22">
         <v>4</v>
@@ -54823,7 +54783,7 @@
         <v>2</v>
       </c>
       <c r="E955" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F955" s="22">
         <v>2</v>
@@ -54889,7 +54849,7 @@
         <v>3</v>
       </c>
       <c r="E956" s="22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F956" s="22">
         <v>1</v>
@@ -54955,7 +54915,7 @@
         <v>2</v>
       </c>
       <c r="E957" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F957" s="22">
         <v>0</v>
@@ -55021,7 +54981,7 @@
         <v>2</v>
       </c>
       <c r="E958" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F958" s="22">
         <v>1</v>
@@ -55080,7 +55040,7 @@
       <c r="B960" s="2"/>
       <c r="C960" s="2"/>
       <c r="D960" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E960" s="3"/>
       <c r="F960" s="3"/>
@@ -55553,7 +55513,7 @@
         <v>3.8</v>
       </c>
       <c r="I969" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J969" s="34"/>
       <c r="K969" s="34">
@@ -56260,7 +56220,7 @@
         <v>5.1079999999999997</v>
       </c>
       <c r="H981" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I981" s="22">
         <v>0</v>
@@ -56300,7 +56260,7 @@
         <v>29</v>
       </c>
       <c r="V981" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="982" spans="1:22">
@@ -56392,7 +56352,7 @@
         <v>9.48</v>
       </c>
       <c r="H983" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I983" s="22">
         <v>0</v>
@@ -56432,7 +56392,7 @@
         <v>27</v>
       </c>
       <c r="V983" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="984" spans="1:22">
@@ -56681,7 +56641,7 @@
         <v>122</v>
       </c>
       <c r="Q987" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="R987" s="22" t="s">
         <v>125</v>
@@ -56706,7 +56666,7 @@
       <c r="B989" s="2"/>
       <c r="C989" s="2"/>
       <c r="D989" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E989" s="3"/>
       <c r="F989" s="3"/>
@@ -57026,41 +56986,41 @@
         <v>2</v>
       </c>
       <c r="B996" s="42" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C996" s="42" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D996" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E996" s="42" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F996" s="42" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G996" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H996" s="42" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I996" s="42" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="J996" s="43"/>
       <c r="K996" s="43" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L996" s="43" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="M996" s="43" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="N996" s="43" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="O996" s="43" t="s">
         <v>120</v>
@@ -57069,22 +57029,22 @@
         <v>129</v>
       </c>
       <c r="Q996" s="42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R996" s="42" t="s">
         <v>123</v>
       </c>
       <c r="S996" s="43" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T996" s="43" t="s">
         <v>126</v>
       </c>
       <c r="U996" s="43" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="V996" s="42" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="997" spans="1:22">
@@ -57199,7 +57159,7 @@
         <v>129</v>
       </c>
       <c r="Q998" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R998" s="22" t="s">
         <v>123</v>
@@ -58863,7 +58823,7 @@
         <v>3</v>
       </c>
       <c r="G1028" s="22" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H1028" s="22">
         <v>2.6</v>
@@ -58879,7 +58839,7 @@
         <v>15.6</v>
       </c>
       <c r="M1028" s="34" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="N1028" s="35">
         <v>3.2</v>
@@ -58995,7 +58955,7 @@
         <v>1</v>
       </c>
       <c r="G1030" s="22" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H1030" s="22">
         <v>3.6</v>
@@ -59023,7 +58983,7 @@
         <v>119</v>
       </c>
       <c r="Q1030" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="R1030" s="22" t="s">
         <v>123</v>
@@ -59375,7 +59335,7 @@
         <v>2</v>
       </c>
       <c r="G1037" s="22" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H1037" s="22">
         <v>3</v>
@@ -59604,7 +59564,7 @@
         <v>123</v>
       </c>
       <c r="R1040" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="S1040" s="34">
         <v>1</v>
@@ -59771,7 +59731,7 @@
         <v>2</v>
       </c>
       <c r="G1043" s="22" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H1043" s="22">
         <v>3.8</v>
@@ -59903,7 +59863,7 @@
         <v>1</v>
       </c>
       <c r="G1045" s="22" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H1045" s="22">
         <v>3.8</v>

</xml_diff>

<commit_message>
Re-adding manually curated data
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2014 data/BogLower5-R3 and R4.xlsx
+++ b/Data/phenotypic data/RawData/2014 data/BogLower5-R3 and R4.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6428" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6439" uniqueCount="213">
   <si>
     <t>Date measured:</t>
   </si>
@@ -455,9 +455,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>R/FUR</t>
   </si>
   <si>
@@ -480,9 +477,6 @@
   </si>
   <si>
     <t>4.793*</t>
-  </si>
-  <si>
-    <t>MS</t>
   </si>
   <si>
     <t>2.89*</t>
@@ -659,9 +653,6 @@
     <t>*Empty bag</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>6.09*</t>
   </si>
   <si>
@@ -675,9 +666,6 @@
   </si>
   <si>
     <t>Date measured: 11/15/14</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>FUR/P</t>
@@ -1324,12 +1312,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:V1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA534" sqref="AA534"/>
+    <sheetView tabSelected="1" topLeftCell="A513" workbookViewId="0">
+      <selection activeCell="V532" sqref="V532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" customWidth="1"/>
+    <col min="14" max="14" width="4.83203125" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="6.5" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" customWidth="1"/>
+    <col min="18" max="18" width="7.1640625" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" customWidth="1"/>
+    <col min="20" max="20" width="6.5" customWidth="1"/>
+    <col min="21" max="21" width="5.83203125" customWidth="1"/>
+    <col min="22" max="22" width="8.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:22" ht="15">
       <c r="A3" s="1" t="s">
@@ -1338,7 +1348,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1613,7 +1623,7 @@
         <v>2.6</v>
       </c>
       <c r="I9" s="22">
-        <v>18.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="J9" s="34"/>
       <c r="K9" s="34">
@@ -1679,7 +1689,7 @@
         <v>4.7</v>
       </c>
       <c r="I10" s="22">
-        <v>20.9</v>
+        <v>0</v>
       </c>
       <c r="J10" s="34"/>
       <c r="K10" s="34">
@@ -1745,7 +1755,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I11" s="22">
-        <v>17.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="J11" s="34"/>
       <c r="K11" s="34">
@@ -1811,7 +1821,7 @@
         <v>2.7</v>
       </c>
       <c r="I12" s="22">
-        <v>18.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="J12" s="34"/>
       <c r="K12" s="34">
@@ -1874,10 +1884,10 @@
         <v>2.52</v>
       </c>
       <c r="H13" s="22">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="I13" s="22">
-        <v>15.6</v>
+        <v>0</v>
       </c>
       <c r="J13" s="34"/>
       <c r="K13" s="34">
@@ -1943,7 +1953,7 @@
         <v>1.3</v>
       </c>
       <c r="I14" s="22">
-        <v>14.3</v>
+        <v>0</v>
       </c>
       <c r="J14" s="34"/>
       <c r="K14" s="34">
@@ -2003,13 +2013,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H15" s="22">
         <v>2.9</v>
       </c>
       <c r="I15" s="38">
-        <v>18.2</v>
+        <v>0</v>
       </c>
       <c r="J15" s="34"/>
       <c r="K15" s="34">
@@ -2069,13 +2079,13 @@
         <v>2</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H16" s="22">
         <v>1.9</v>
       </c>
       <c r="I16" s="22">
-        <v>19.8</v>
+        <v>0</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34">
@@ -2141,7 +2151,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="22">
-        <v>18.399999999999999</v>
+        <v>0</v>
       </c>
       <c r="J17" s="34"/>
       <c r="K17" s="34">
@@ -2207,7 +2217,7 @@
         <v>2.7</v>
       </c>
       <c r="I18" s="22">
-        <v>20.6</v>
+        <v>1.7</v>
       </c>
       <c r="J18" s="34"/>
       <c r="K18" s="34">
@@ -2377,13 +2387,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="22">
         <v>0</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H22" s="22">
         <v>4</v>
@@ -2411,7 +2421,7 @@
         <v>119</v>
       </c>
       <c r="Q22" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R22" s="22" t="s">
         <v>123</v>
@@ -2575,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" s="22">
         <v>2</v>
@@ -2641,7 +2651,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="22">
         <v>1</v>
@@ -2675,7 +2685,7 @@
         <v>122</v>
       </c>
       <c r="Q26" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R26" s="22" t="s">
         <v>124</v>
@@ -2839,13 +2849,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="22">
         <v>1</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H29" s="22">
         <v>2.2999999999999998</v>
@@ -2873,7 +2883,7 @@
         <v>122</v>
       </c>
       <c r="Q29" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R29" s="22" t="s">
         <v>124</v>
@@ -2964,7 +2974,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -3732,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="T45" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U45" s="34">
         <v>7</v>
@@ -4593,7 +4603,7 @@
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -4956,7 +4966,7 @@
         <v>119</v>
       </c>
       <c r="Q68" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R68" s="22" t="s">
         <v>124</v>
@@ -4994,7 +5004,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H69" s="22">
         <v>2.4</v>
@@ -5022,7 +5032,7 @@
         <v>129</v>
       </c>
       <c r="Q69" s="22" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="R69" s="22" t="s">
         <v>124</v>
@@ -5088,7 +5098,7 @@
         <v>129</v>
       </c>
       <c r="Q70" s="22" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="R70" s="22" t="s">
         <v>124</v>
@@ -5126,7 +5136,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H71" s="22">
         <v>0</v>
@@ -5286,7 +5296,7 @@
         <v>129</v>
       </c>
       <c r="Q73" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R73" s="22" t="s">
         <v>124</v>
@@ -5456,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="G76" s="22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H76" s="22">
         <v>4.2</v>
@@ -5484,7 +5494,7 @@
         <v>119</v>
       </c>
       <c r="Q76" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R76" s="22" t="s">
         <v>124</v>
@@ -5668,7 +5678,7 @@
         <v>119</v>
       </c>
       <c r="Q80" s="22" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="R80" s="22" t="s">
         <v>124</v>
@@ -5955,7 +5965,7 @@
         <v>7</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C85" s="22"/>
       <c r="D85" s="22"/>
@@ -6186,7 +6196,7 @@
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -6590,7 +6600,7 @@
         <v>3.16</v>
       </c>
       <c r="H98" s="22">
-        <v>21</v>
+        <v>2.1</v>
       </c>
       <c r="I98" s="22">
         <v>0</v>
@@ -6785,7 +6795,7 @@
         <v>1</v>
       </c>
       <c r="G101" s="22" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H101" s="22">
         <v>4.8</v>
@@ -7812,7 +7822,7 @@
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
@@ -8307,7 +8317,7 @@
         <v>119</v>
       </c>
       <c r="Q128" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R128" s="22" t="s">
         <v>124</v>
@@ -8700,7 +8710,7 @@
         <v>138</v>
       </c>
       <c r="P134" s="37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q134" s="22" t="s">
         <v>124</v>
@@ -10775,7 +10785,7 @@
         <v>119</v>
       </c>
       <c r="Q171" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R171" s="22" t="s">
         <v>124</v>
@@ -10907,7 +10917,7 @@
         <v>119</v>
       </c>
       <c r="Q173" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R173" s="22" t="s">
         <v>124</v>
@@ -10973,7 +10983,7 @@
         <v>122</v>
       </c>
       <c r="Q174" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R174" s="22" t="s">
         <v>124</v>
@@ -14261,7 +14271,7 @@
         <v>0</v>
       </c>
       <c r="G233" s="22" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H233" s="22">
         <v>5</v>
@@ -15811,7 +15821,7 @@
         <v>2</v>
       </c>
       <c r="G261" s="22">
-        <v>7078</v>
+        <v>7.78</v>
       </c>
       <c r="H261" s="22">
         <v>5</v>
@@ -15842,7 +15852,7 @@
         <v>124</v>
       </c>
       <c r="R261" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S261" s="34">
         <v>1</v>
@@ -15930,7 +15940,7 @@
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E264" s="3"/>
       <c r="F264" s="3"/>
@@ -16278,7 +16288,7 @@
         <v>17.2</v>
       </c>
       <c r="L271" s="34">
-        <v>41.8</v>
+        <v>14.8</v>
       </c>
       <c r="M271" s="34">
         <v>1.651</v>
@@ -17069,7 +17079,7 @@
         <v>129</v>
       </c>
       <c r="Q284" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R284" s="22" t="s">
         <v>124</v>
@@ -17333,7 +17343,7 @@
         <v>119</v>
       </c>
       <c r="Q288" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R288" s="22" t="s">
         <v>124</v>
@@ -17465,7 +17475,7 @@
         <v>119</v>
       </c>
       <c r="Q290" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R290" s="22" t="s">
         <v>124</v>
@@ -17556,7 +17566,7 @@
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E293" s="3"/>
       <c r="F293" s="3"/>
@@ -18438,7 +18448,7 @@
         <v>2.06</v>
       </c>
       <c r="N308" s="35">
-        <v>2.06</v>
+        <v>2.7</v>
       </c>
       <c r="O308" s="37" t="s">
         <v>119</v>
@@ -18827,7 +18837,7 @@
         <v>122</v>
       </c>
       <c r="Q315" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R315" s="22" t="s">
         <v>131</v>
@@ -18836,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="T315" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U315" s="34">
         <v>18</v>
@@ -19100,7 +19110,7 @@
         <v>1</v>
       </c>
       <c r="T319" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U319" s="34">
         <v>28</v>
@@ -19614,7 +19624,7 @@
         <v>124</v>
       </c>
       <c r="R330" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S330" s="34">
         <v>3</v>
@@ -20203,7 +20213,9 @@
       <c r="U340" s="34">
         <v>25</v>
       </c>
-      <c r="V340" s="22"/>
+      <c r="V340" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="341" spans="1:22">
       <c r="A341" s="4">
@@ -20267,7 +20279,9 @@
       <c r="U341" s="34">
         <v>29</v>
       </c>
-      <c r="V341" s="22"/>
+      <c r="V341" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="342" spans="1:22">
       <c r="A342" s="4">
@@ -20331,7 +20345,9 @@
       <c r="U342" s="34">
         <v>10</v>
       </c>
-      <c r="V342" s="22"/>
+      <c r="V342" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="343" spans="1:22">
       <c r="A343" s="4">
@@ -20395,7 +20411,9 @@
       <c r="U343" s="34">
         <v>19</v>
       </c>
-      <c r="V343" s="22"/>
+      <c r="V343" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="344" spans="1:22">
       <c r="A344" s="4">
@@ -20459,7 +20477,9 @@
       <c r="U344" s="34">
         <v>13</v>
       </c>
-      <c r="V344" s="22"/>
+      <c r="V344" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="345" spans="1:22">
       <c r="A345" s="4">
@@ -20523,7 +20543,9 @@
       <c r="U345" s="34">
         <v>20</v>
       </c>
-      <c r="V345" s="22"/>
+      <c r="V345" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="346" spans="1:22">
       <c r="A346" s="4">
@@ -20587,7 +20609,9 @@
       <c r="U346" s="34">
         <v>21</v>
       </c>
-      <c r="V346" s="22"/>
+      <c r="V346" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="347" spans="1:22">
       <c r="A347" s="4">
@@ -20651,7 +20675,9 @@
       <c r="U347" s="34">
         <v>22</v>
       </c>
-      <c r="V347" s="22"/>
+      <c r="V347" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="348" spans="1:22">
       <c r="A348" s="4">
@@ -20715,7 +20741,9 @@
       <c r="U348" s="34">
         <v>24</v>
       </c>
-      <c r="V348" s="22"/>
+      <c r="V348" s="22" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="349" spans="1:22">
       <c r="A349" s="4">
@@ -20765,7 +20793,7 @@
         <v>119</v>
       </c>
       <c r="Q349" s="22" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="R349" s="22" t="s">
         <v>124</v>
@@ -20779,9 +20807,14 @@
       <c r="U349" s="34">
         <v>17</v>
       </c>
-      <c r="V349" s="22"/>
+      <c r="V349" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="350" spans="1:22">
+      <c r="A350" s="4">
+        <v>11</v>
+      </c>
       <c r="B350" s="22">
         <v>5</v>
       </c>
@@ -20838,6 +20871,9 @@
       </c>
       <c r="U350" s="34">
         <v>15</v>
+      </c>
+      <c r="V350" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="351" spans="1:22" ht="15">
@@ -21144,7 +21180,7 @@
         <v>119</v>
       </c>
       <c r="Q357" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R357" s="22" t="s">
         <v>124</v>
@@ -21210,7 +21246,7 @@
         <v>119</v>
       </c>
       <c r="Q358" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R358" s="22" t="s">
         <v>124</v>
@@ -21276,7 +21312,7 @@
         <v>119</v>
       </c>
       <c r="Q359" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R359" s="22" t="s">
         <v>124</v>
@@ -21342,7 +21378,7 @@
         <v>119</v>
       </c>
       <c r="Q360" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R360" s="22" t="s">
         <v>124</v>
@@ -21408,7 +21444,7 @@
         <v>119</v>
       </c>
       <c r="Q361" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R361" s="22" t="s">
         <v>131</v>
@@ -21474,7 +21510,7 @@
         <v>119</v>
       </c>
       <c r="Q362" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R362" s="22" t="s">
         <v>124</v>
@@ -21483,7 +21519,7 @@
         <v>2</v>
       </c>
       <c r="T362" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U362" s="34">
         <v>21</v>
@@ -21540,7 +21576,7 @@
         <v>119</v>
       </c>
       <c r="Q363" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R363" s="22" t="s">
         <v>124</v>
@@ -21606,7 +21642,7 @@
         <v>119</v>
       </c>
       <c r="Q364" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R364" s="22" t="s">
         <v>124</v>
@@ -21672,7 +21708,7 @@
         <v>122</v>
       </c>
       <c r="Q365" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R365" s="22" t="s">
         <v>124</v>
@@ -21747,7 +21783,7 @@
         <v>1</v>
       </c>
       <c r="T366" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U366" s="34">
         <v>9</v>
@@ -22473,7 +22509,7 @@
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E380" s="3"/>
       <c r="F380" s="3"/>
@@ -24099,7 +24135,7 @@
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
       <c r="D409" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E409" s="3"/>
       <c r="F409" s="3"/>
@@ -24660,7 +24696,7 @@
         <v>120</v>
       </c>
       <c r="Q419" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R419" s="22" t="s">
         <v>124</v>
@@ -24990,7 +25026,7 @@
         <v>122</v>
       </c>
       <c r="Q424" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R424" s="22" t="s">
         <v>124</v>
@@ -25121,7 +25157,7 @@
         <v>16</v>
       </c>
       <c r="V427" s="22" t="s">
-        <v>214</v>
+        <v>128</v>
       </c>
     </row>
     <row r="428" spans="1:22">
@@ -25187,7 +25223,7 @@
         <v>24</v>
       </c>
       <c r="V428" s="22" t="s">
-        <v>214</v>
+        <v>128</v>
       </c>
     </row>
     <row r="429" spans="1:22">
@@ -25385,7 +25421,7 @@
         <v>17</v>
       </c>
       <c r="V431" s="22" t="s">
-        <v>214</v>
+        <v>128</v>
       </c>
     </row>
     <row r="432" spans="1:22">
@@ -25451,7 +25487,7 @@
         <v>10</v>
       </c>
       <c r="V432" s="22" t="s">
-        <v>214</v>
+        <v>128</v>
       </c>
     </row>
     <row r="433" spans="1:22">
@@ -25725,7 +25761,7 @@
       <c r="B438" s="2"/>
       <c r="C438" s="2"/>
       <c r="D438" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E438" s="3"/>
       <c r="F438" s="3"/>
@@ -26091,7 +26127,7 @@
         <v>124</v>
       </c>
       <c r="R445" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S445">
         <v>1</v>
@@ -26553,7 +26589,7 @@
         <v>124</v>
       </c>
       <c r="R452" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S452">
         <v>1</v>
@@ -27351,7 +27387,7 @@
       <c r="B467" s="2"/>
       <c r="C467" s="2"/>
       <c r="D467" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E467" s="3"/>
       <c r="F467" s="3"/>
@@ -27648,7 +27684,7 @@
         <v>119</v>
       </c>
       <c r="Q473" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R473" s="22" t="s">
         <v>124</v>
@@ -27780,7 +27816,7 @@
         <v>119</v>
       </c>
       <c r="Q475" s="22" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="R475" s="22" t="s">
         <v>124</v>
@@ -27789,7 +27825,7 @@
         <v>1</v>
       </c>
       <c r="T475" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U475" s="34">
         <v>20</v>
@@ -27987,7 +28023,7 @@
         <v>1</v>
       </c>
       <c r="T478" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U478" s="34">
         <v>15</v>
@@ -28119,7 +28155,7 @@
         <v>1</v>
       </c>
       <c r="T480" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U480" s="34">
         <v>9</v>
@@ -28185,7 +28221,7 @@
         <v>2</v>
       </c>
       <c r="T481" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U481" s="34">
         <v>14</v>
@@ -28242,7 +28278,7 @@
         <v>122</v>
       </c>
       <c r="Q482" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R482" s="22" t="s">
         <v>124</v>
@@ -28251,7 +28287,7 @@
         <v>2</v>
       </c>
       <c r="T482" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U482" s="34">
         <v>15</v>
@@ -28435,7 +28471,7 @@
         <v>121</v>
       </c>
       <c r="U486" s="34">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="V486" s="22" t="s">
         <v>127</v>
@@ -28530,7 +28566,7 @@
         <v>4.29</v>
       </c>
       <c r="H488" s="22">
-        <v>3.2</v>
+        <v>3.7</v>
       </c>
       <c r="I488" s="22">
         <v>0</v>
@@ -28976,7 +29012,7 @@
       <c r="B496" s="2"/>
       <c r="C496" s="2"/>
       <c r="D496" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E496" s="3"/>
       <c r="F496" s="3"/>
@@ -29414,7 +29450,7 @@
         <v>1</v>
       </c>
       <c r="T504" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U504" s="34">
         <v>8</v>
@@ -29678,7 +29714,7 @@
         <v>1</v>
       </c>
       <c r="T508" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U508" s="34">
         <v>25</v>
@@ -29789,7 +29825,7 @@
         <v>16.3</v>
       </c>
       <c r="M510" s="34">
-        <v>2.31</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="N510" s="35">
         <v>3.3</v>
@@ -30454,7 +30490,7 @@
         <v>1</v>
       </c>
       <c r="T521" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U521" s="34">
         <v>16</v>
@@ -30827,7 +30863,7 @@
     </row>
     <row r="530" spans="1:22">
       <c r="A530" s="28" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B530" s="29"/>
       <c r="C530" s="29"/>
@@ -31298,7 +31334,7 @@
         <v>124</v>
       </c>
       <c r="R537" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="S537" s="34">
         <v>1</v>
@@ -35813,13 +35849,13 @@
         <v>2.9</v>
       </c>
       <c r="O618" s="36" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P618" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q618" s="22" t="s">
-        <v>125</v>
+        <v>207</v>
       </c>
       <c r="R618" s="22" t="s">
         <v>124</v>
@@ -35879,10 +35915,10 @@
         <v>3.7</v>
       </c>
       <c r="O619" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P619" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q619" s="22" t="s">
         <v>123</v>
@@ -35923,7 +35959,7 @@
         <v>6</v>
       </c>
       <c r="G620" s="22">
-        <v>2.3210000000000002</v>
+        <v>2.5209999999999999</v>
       </c>
       <c r="H620" s="22">
         <v>3.1</v>
@@ -35945,10 +35981,10 @@
         <v>3.3</v>
       </c>
       <c r="O620" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P620" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q620" s="22" t="s">
         <v>123</v>
@@ -36011,10 +36047,10 @@
         <v>3.1</v>
       </c>
       <c r="O621" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P621" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q621" s="22" t="s">
         <v>123</v>
@@ -36077,10 +36113,10 @@
         <v>3</v>
       </c>
       <c r="O622" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P622" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="Q622" s="22" t="s">
         <v>125</v>
@@ -36143,10 +36179,10 @@
         <v>2.9</v>
       </c>
       <c r="O623" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P623" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="Q623" s="22" t="s">
         <v>123</v>
@@ -36209,10 +36245,10 @@
         <v>2.8</v>
       </c>
       <c r="O624" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P624" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="Q624" s="22" t="s">
         <v>123</v>
@@ -36275,10 +36311,10 @@
         <v>3.1</v>
       </c>
       <c r="O625" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P625" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q625" s="22" t="s">
         <v>125</v>
@@ -36341,10 +36377,10 @@
         <v>2.8</v>
       </c>
       <c r="O626" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P626" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="Q626" s="22" t="s">
         <v>123</v>
@@ -36407,16 +36443,16 @@
         <v>3.5</v>
       </c>
       <c r="O627" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P627" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q627" s="22" t="s">
         <v>125</v>
       </c>
       <c r="R627" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S627" s="34">
         <v>2</v>
@@ -36529,7 +36565,7 @@
         <v>119</v>
       </c>
       <c r="Q630" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R630" s="22" t="s">
         <v>131</v>
@@ -36793,7 +36829,7 @@
         <v>122</v>
       </c>
       <c r="Q634" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R634" s="22" t="s">
         <v>124</v>
@@ -37148,7 +37184,7 @@
       <c r="B641" s="2"/>
       <c r="C641" s="2"/>
       <c r="D641" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E641" s="3"/>
       <c r="F641" s="3"/>
@@ -37520,7 +37556,7 @@
         <v>2</v>
       </c>
       <c r="T648" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U648" s="34">
         <v>6</v>
@@ -37559,7 +37595,7 @@
       </c>
       <c r="J649" s="34"/>
       <c r="K649" s="34">
-        <v>1.94</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="L649" s="34">
         <v>15.6</v>
@@ -37586,7 +37622,7 @@
         <v>2</v>
       </c>
       <c r="T649" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U649" s="34">
         <v>3</v>
@@ -37652,7 +37688,7 @@
         <v>1</v>
       </c>
       <c r="T650" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U650" s="34">
         <v>10</v>
@@ -37718,7 +37754,7 @@
         <v>2</v>
       </c>
       <c r="T651" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U651" s="34">
         <v>10</v>
@@ -37916,7 +37952,7 @@
         <v>2</v>
       </c>
       <c r="T654" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U654" s="34">
         <v>6</v>
@@ -37982,7 +38018,7 @@
         <v>3</v>
       </c>
       <c r="T655" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U655" s="34">
         <v>16</v>
@@ -38065,7 +38101,9 @@
       <c r="E657" s="11"/>
       <c r="F657" s="11"/>
       <c r="G657" s="11"/>
-      <c r="H657" s="11"/>
+      <c r="H657" s="11">
+        <v>3.9</v>
+      </c>
       <c r="I657" s="11"/>
       <c r="J657" s="16"/>
       <c r="K657" s="16"/>
@@ -38410,7 +38448,7 @@
         <v>3.508</v>
       </c>
       <c r="N663" s="35">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="O663" s="37" t="s">
         <v>119</v>
@@ -38774,7 +38812,7 @@
       <c r="B670" s="2"/>
       <c r="C670" s="2"/>
       <c r="D670" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E670" s="3"/>
       <c r="F670" s="3"/>
@@ -39691,7 +39729,9 @@
       <c r="E686" s="11"/>
       <c r="F686" s="11"/>
       <c r="G686" s="11"/>
-      <c r="H686" s="11"/>
+      <c r="H686" s="11">
+        <v>2.4</v>
+      </c>
       <c r="I686" s="11"/>
       <c r="J686" s="16"/>
       <c r="K686" s="16"/>
@@ -39885,7 +39925,7 @@
         <v>0</v>
       </c>
       <c r="G690" s="22">
-        <v>4.0419999999999998</v>
+        <v>4.6420000000000003</v>
       </c>
       <c r="H690" s="22">
         <v>2.4</v>
@@ -40027,7 +40067,7 @@
       </c>
       <c r="J692" s="34"/>
       <c r="K692" s="34">
-        <v>21.4</v>
+        <v>24.6</v>
       </c>
       <c r="L692" s="34">
         <v>19.899999999999999</v>
@@ -40309,7 +40349,7 @@
         <v>119</v>
       </c>
       <c r="Q696" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R696" s="22" t="s">
         <v>124</v>
@@ -40400,7 +40440,7 @@
       <c r="B699" s="2"/>
       <c r="C699" s="2"/>
       <c r="D699" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E699" s="3"/>
       <c r="F699" s="3"/>
@@ -41379,7 +41419,7 @@
         <v>3</v>
       </c>
       <c r="G717" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H717" s="22">
         <v>3.8</v>
@@ -41602,7 +41642,7 @@
         <v>120</v>
       </c>
       <c r="P720" s="37" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="Q720" s="22" t="s">
         <v>124</v>
@@ -41788,7 +41828,7 @@
         <v>23.2</v>
       </c>
       <c r="L723" s="34">
-        <v>15.7</v>
+        <v>15.9</v>
       </c>
       <c r="M723" s="34">
         <v>2.528</v>
@@ -42026,7 +42066,7 @@
       <c r="B728" s="2"/>
       <c r="C728" s="2"/>
       <c r="D728" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E728" s="3"/>
       <c r="F728" s="3"/>
@@ -42596,7 +42636,7 @@
         <v>1</v>
       </c>
       <c r="T738" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="U738" s="34">
         <v>32</v>
@@ -42662,7 +42702,7 @@
         <v>1</v>
       </c>
       <c r="T739" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="U739" s="34">
         <v>23</v>
@@ -43005,7 +43045,7 @@
         <v>2</v>
       </c>
       <c r="G746" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H746" s="22">
         <v>2.7</v>
@@ -43027,10 +43067,10 @@
         <v>2.5</v>
       </c>
       <c r="O746" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P746" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="Q746" s="22" t="s">
         <v>124</v>
@@ -43071,7 +43111,7 @@
         <v>2</v>
       </c>
       <c r="G747" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H747" s="22">
         <v>4.0999999999999996</v>
@@ -43093,10 +43133,10 @@
         <v>3.2</v>
       </c>
       <c r="O747" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P747" s="37" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="Q747" s="22" t="s">
         <v>124</v>
@@ -43159,7 +43199,7 @@
         <v>2.9</v>
       </c>
       <c r="O748" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P748" s="37" t="s">
         <v>119</v>
@@ -43225,7 +43265,7 @@
         <v>2.6</v>
       </c>
       <c r="O749" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P749" s="37" t="s">
         <v>119</v>
@@ -43282,7 +43322,7 @@
         <v>20.6</v>
       </c>
       <c r="L750" s="34">
-        <v>17.100000000000001</v>
+        <v>17.7</v>
       </c>
       <c r="M750" s="34">
         <v>2.37</v>
@@ -43291,7 +43331,7 @@
         <v>3</v>
       </c>
       <c r="O750" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P750" s="37" t="s">
         <v>119</v>
@@ -43357,7 +43397,7 @@
         <v>2.4</v>
       </c>
       <c r="O751" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P751" s="37" t="s">
         <v>129</v>
@@ -43423,7 +43463,7 @@
         <v>2.6</v>
       </c>
       <c r="O752" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P752" s="37" t="s">
         <v>119</v>
@@ -43489,7 +43529,7 @@
         <v>2.6</v>
       </c>
       <c r="O753" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P753" s="37" t="s">
         <v>119</v>
@@ -43555,7 +43595,7 @@
         <v>3.1</v>
       </c>
       <c r="O754" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P754" s="37" t="s">
         <v>122</v>
@@ -43621,7 +43661,7 @@
         <v>2.7</v>
       </c>
       <c r="O755" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P755" s="37" t="s">
         <v>119</v>
@@ -43652,7 +43692,7 @@
       <c r="B757" s="2"/>
       <c r="C757" s="2"/>
       <c r="D757" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E757" s="3"/>
       <c r="F757" s="3"/>
@@ -43921,7 +43961,7 @@
         <v>0</v>
       </c>
       <c r="G763" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H763" s="22">
         <v>4</v>
@@ -44185,7 +44225,7 @@
         <v>1</v>
       </c>
       <c r="G767" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H767" s="22">
         <v>2.5</v>
@@ -44964,7 +45004,7 @@
         <v>8.125</v>
       </c>
       <c r="H780" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I780" s="22">
         <v>0</v>
@@ -45004,7 +45044,7 @@
         <v>13</v>
       </c>
       <c r="V780" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="781" spans="1:22">
@@ -45225,7 +45265,7 @@
         <v>2</v>
       </c>
       <c r="G784" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H784" s="22">
         <v>3.9</v>
@@ -45278,7 +45318,7 @@
       <c r="B786" s="2"/>
       <c r="C786" s="2"/>
       <c r="D786" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E786" s="3"/>
       <c r="F786" s="3"/>
@@ -46279,7 +46319,7 @@
         <v>2.9</v>
       </c>
       <c r="O804" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P804" s="37" t="s">
         <v>122</v>
@@ -46345,7 +46385,7 @@
         <v>2.8</v>
       </c>
       <c r="O805" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P805" s="37" t="s">
         <v>119</v>
@@ -46405,13 +46445,13 @@
         <v>18.100000000000001</v>
       </c>
       <c r="M806" s="34">
-        <v>2.68</v>
+        <v>2.69</v>
       </c>
       <c r="N806" s="35">
         <v>3.4</v>
       </c>
       <c r="O806" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P806" s="37" t="s">
         <v>122</v>
@@ -46477,7 +46517,7 @@
         <v>3.2</v>
       </c>
       <c r="O807" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P807" s="37" t="s">
         <v>122</v>
@@ -46543,7 +46583,7 @@
         <v>2.9</v>
       </c>
       <c r="O808" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P808" s="37" t="s">
         <v>122</v>
@@ -46609,7 +46649,7 @@
         <v>3.1</v>
       </c>
       <c r="O809" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P809" s="37" t="s">
         <v>119</v>
@@ -46675,7 +46715,7 @@
         <v>3.1</v>
       </c>
       <c r="O810" s="37" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="P810" s="37" t="s">
         <v>122</v>
@@ -46729,7 +46769,7 @@
       </c>
       <c r="J811" s="34"/>
       <c r="K811" s="34">
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="L811" s="34">
         <v>16.8</v>
@@ -46741,7 +46781,7 @@
         <v>3.1</v>
       </c>
       <c r="O811" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P811" s="37" t="s">
         <v>122</v>
@@ -46807,7 +46847,7 @@
         <v>3.3</v>
       </c>
       <c r="O812" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P812" s="37" t="s">
         <v>122</v>
@@ -46851,7 +46891,7 @@
         <v>0</v>
       </c>
       <c r="G813" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H813" s="11">
         <v>2.7</v>
@@ -46867,13 +46907,13 @@
         <v>14.9</v>
       </c>
       <c r="M813" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N813" s="35">
         <v>2.9</v>
       </c>
       <c r="O813" s="37" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="P813" s="37" t="s">
         <v>122</v>
@@ -46907,7 +46947,7 @@
       <c r="B815" s="2"/>
       <c r="C815" s="2"/>
       <c r="D815" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E815" s="3"/>
       <c r="F815" s="3"/>
@@ -47339,7 +47379,7 @@
         <v>123</v>
       </c>
       <c r="R823" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S823" s="34">
         <v>2</v>
@@ -47537,7 +47577,7 @@
         <v>123</v>
       </c>
       <c r="R826" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S826" s="34">
         <v>2</v>
@@ -48348,7 +48388,7 @@
         <v>1</v>
       </c>
       <c r="G840" s="22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H840" s="22">
         <v>3.8</v>
@@ -48533,7 +48573,7 @@
       <c r="B844" s="2"/>
       <c r="C844" s="2"/>
       <c r="D844" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E844" s="3"/>
       <c r="F844" s="3"/>
@@ -48871,7 +48911,7 @@
         <v>4.6210000000000004</v>
       </c>
       <c r="H851" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I851" s="22">
         <v>0</v>
@@ -48911,7 +48951,7 @@
         <v>7</v>
       </c>
       <c r="V851" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="852" spans="1:22">
@@ -48977,7 +49017,7 @@
         <v>16</v>
       </c>
       <c r="V852" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="853" spans="1:22">
@@ -49043,7 +49083,7 @@
         <v>11</v>
       </c>
       <c r="V853" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="854" spans="1:22">
@@ -49132,7 +49172,7 @@
         <v>1</v>
       </c>
       <c r="G855" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H855" s="22">
         <v>4.0999999999999996</v>
@@ -49175,7 +49215,7 @@
         <v>11</v>
       </c>
       <c r="V855" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="856" spans="1:22">
@@ -49333,7 +49373,7 @@
         <v>6.9320000000000004</v>
       </c>
       <c r="H858" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I858" s="22">
         <v>0</v>
@@ -49373,7 +49413,7 @@
         <v>17</v>
       </c>
       <c r="V858" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="859" spans="1:22">
@@ -50159,7 +50199,7 @@
       <c r="B873" s="2"/>
       <c r="C873" s="2"/>
       <c r="D873" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E873" s="3"/>
       <c r="F873" s="3"/>
@@ -50890,7 +50930,7 @@
         <v>0</v>
       </c>
       <c r="G886" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H886" s="22">
         <v>4.5</v>
@@ -50906,7 +50946,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="M886" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N886" s="22">
         <v>2.8</v>
@@ -51402,7 +51442,7 @@
         <v>1</v>
       </c>
       <c r="G895" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H895" s="22">
         <v>4.8</v>
@@ -51788,7 +51828,7 @@
       <c r="B902" s="2"/>
       <c r="C902" s="2"/>
       <c r="D902" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E902" s="3"/>
       <c r="F902" s="3"/>
@@ -52060,7 +52100,7 @@
         <v>6.48</v>
       </c>
       <c r="H908" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I908" s="22">
         <v>0</v>
@@ -52151,7 +52191,7 @@
         <v>122</v>
       </c>
       <c r="Q909" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R909" s="22" t="s">
         <v>123</v>
@@ -52205,7 +52245,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="M910" s="34">
-        <v>1.26</v>
+        <v>2.16</v>
       </c>
       <c r="N910" s="35">
         <v>3</v>
@@ -53053,7 +53093,7 @@
         <v>3</v>
       </c>
       <c r="O924" s="37" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="P924" s="37" t="s">
         <v>122</v>
@@ -53414,7 +53454,7 @@
       <c r="B931" s="2"/>
       <c r="C931" s="2"/>
       <c r="D931" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E931" s="3"/>
       <c r="F931" s="3"/>
@@ -54387,7 +54427,7 @@
         <v>2</v>
       </c>
       <c r="E949" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F949" s="22">
         <v>3</v>
@@ -54453,7 +54493,7 @@
         <v>2</v>
       </c>
       <c r="E950" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F950" s="22">
         <v>1</v>
@@ -54519,7 +54559,7 @@
         <v>2</v>
       </c>
       <c r="E951" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F951" s="22">
         <v>4</v>
@@ -54585,7 +54625,7 @@
         <v>4</v>
       </c>
       <c r="E952" s="22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F952" s="22">
         <v>3</v>
@@ -54651,7 +54691,7 @@
         <v>2</v>
       </c>
       <c r="E953" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F953" s="22">
         <v>1</v>
@@ -54717,7 +54757,7 @@
         <v>3</v>
       </c>
       <c r="E954" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F954" s="22">
         <v>4</v>
@@ -54783,7 +54823,7 @@
         <v>2</v>
       </c>
       <c r="E955" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F955" s="22">
         <v>2</v>
@@ -54849,7 +54889,7 @@
         <v>3</v>
       </c>
       <c r="E956" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F956" s="22">
         <v>1</v>
@@ -54915,7 +54955,7 @@
         <v>2</v>
       </c>
       <c r="E957" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F957" s="22">
         <v>0</v>
@@ -54981,7 +55021,7 @@
         <v>2</v>
       </c>
       <c r="E958" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F958" s="22">
         <v>1</v>
@@ -55040,7 +55080,7 @@
       <c r="B960" s="2"/>
       <c r="C960" s="2"/>
       <c r="D960" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E960" s="3"/>
       <c r="F960" s="3"/>
@@ -55513,7 +55553,7 @@
         <v>3.8</v>
       </c>
       <c r="I969" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J969" s="34"/>
       <c r="K969" s="34">
@@ -56220,7 +56260,7 @@
         <v>5.1079999999999997</v>
       </c>
       <c r="H981" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I981" s="22">
         <v>0</v>
@@ -56260,7 +56300,7 @@
         <v>29</v>
       </c>
       <c r="V981" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="982" spans="1:22">
@@ -56352,7 +56392,7 @@
         <v>9.48</v>
       </c>
       <c r="H983" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I983" s="22">
         <v>0</v>
@@ -56392,7 +56432,7 @@
         <v>27</v>
       </c>
       <c r="V983" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="984" spans="1:22">
@@ -56641,7 +56681,7 @@
         <v>122</v>
       </c>
       <c r="Q987" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R987" s="22" t="s">
         <v>125</v>
@@ -56666,7 +56706,7 @@
       <c r="B989" s="2"/>
       <c r="C989" s="2"/>
       <c r="D989" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E989" s="3"/>
       <c r="F989" s="3"/>
@@ -56986,41 +57026,41 @@
         <v>2</v>
       </c>
       <c r="B996" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C996" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D996" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="C996" s="42" t="s">
+      <c r="E996" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="D996" s="42" t="s">
+      <c r="F996" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="E996" s="42" t="s">
+      <c r="G996" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="F996" s="42" t="s">
+      <c r="H996" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="G996" s="42" t="s">
+      <c r="I996" s="42" t="s">
         <v>182</v>
-      </c>
-      <c r="H996" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="I996" s="42" t="s">
-        <v>184</v>
       </c>
       <c r="J996" s="43"/>
       <c r="K996" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="L996" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="M996" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="L996" s="43" t="s">
+      <c r="N996" s="43" t="s">
         <v>186</v>
-      </c>
-      <c r="M996" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="N996" s="43" t="s">
-        <v>188</v>
       </c>
       <c r="O996" s="43" t="s">
         <v>120</v>
@@ -57029,22 +57069,22 @@
         <v>129</v>
       </c>
       <c r="Q996" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R996" s="42" t="s">
         <v>123</v>
       </c>
       <c r="S996" s="43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T996" s="43" t="s">
         <v>126</v>
       </c>
       <c r="U996" s="43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="V996" s="42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="997" spans="1:22">
@@ -57159,7 +57199,7 @@
         <v>129</v>
       </c>
       <c r="Q998" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R998" s="22" t="s">
         <v>123</v>
@@ -58823,7 +58863,7 @@
         <v>3</v>
       </c>
       <c r="G1028" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H1028" s="22">
         <v>2.6</v>
@@ -58839,7 +58879,7 @@
         <v>15.6</v>
       </c>
       <c r="M1028" s="34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N1028" s="35">
         <v>3.2</v>
@@ -58955,7 +58995,7 @@
         <v>1</v>
       </c>
       <c r="G1030" s="22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H1030" s="22">
         <v>3.6</v>
@@ -58983,7 +59023,7 @@
         <v>119</v>
       </c>
       <c r="Q1030" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R1030" s="22" t="s">
         <v>123</v>
@@ -59335,7 +59375,7 @@
         <v>2</v>
       </c>
       <c r="G1037" s="22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H1037" s="22">
         <v>3</v>
@@ -59564,7 +59604,7 @@
         <v>123</v>
       </c>
       <c r="R1040" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S1040" s="34">
         <v>1</v>
@@ -59731,7 +59771,7 @@
         <v>2</v>
       </c>
       <c r="G1043" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H1043" s="22">
         <v>3.8</v>
@@ -59863,7 +59903,7 @@
         <v>1</v>
       </c>
       <c r="G1045" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H1045" s="22">
         <v>3.8</v>

</xml_diff>